<commit_message>
adding logindata Excel Utility
</commit_message>
<xml_diff>
--- a/OfflineWebsite/src/test/resources/Data.xlsx
+++ b/OfflineWebsite/src/test/resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akshay S Jain\git\OfflineWebsite\OfflineWebsite\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D9B285-B5BA-4BAD-A805-0D747C27B74E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7ABDF22-873E-410B-8CC5-65735642C5AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginWithHeading" sheetId="1" r:id="rId1"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1445,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523813A9-4AB2-4F99-9449-1F790C9F5E8D}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>